<commit_message>
the test was sucessful, whole prpvess seems finished.
</commit_message>
<xml_diff>
--- a/simulation/ML-DSA-65_DSA_elapsed_time_parallel.xlsx
+++ b/simulation/ML-DSA-65_DSA_elapsed_time_parallel.xlsx
@@ -320,90 +320,90 @@
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B1">
-        <v>0.045689921</v>
+        <v>0.101622015</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>0.045888488</v>
+        <v>0.102195086</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.047965597</v>
+        <v>0.101268767</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0.052870394</v>
+        <v>0.102202233</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.052581754</v>
+        <v>0.102285665</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>0.056684705</v>
+        <v>0.102706123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>0.057045839</v>
+        <v>0.102763022</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>0.05823884</v>
+        <v>0.102627419</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>0.058591214</v>
+        <v>0.102263281</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>0.058638981</v>
+        <v>0.102889773</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>0.06299479</v>
+        <v>0.021710895</v>
       </c>
     </row>
     <row r="12">
@@ -411,479 +411,479 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>0.073046946</v>
+        <v>0.022506369</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>0.073433743</v>
+        <v>0.033151039</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14">
-        <v>0.073685349</v>
+        <v>0.030813866</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>0.073708148</v>
+        <v>0.036838368</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>0.08854889</v>
+        <v>0.036610519</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>0.09022569</v>
+        <v>0.037473588</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>0.090096288</v>
+        <v>0.036646144</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>0.091439145</v>
+        <v>0.038445264</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20">
-        <v>0.094155027</v>
+        <v>0.035702295</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>0.094597999</v>
+        <v>0.035256481</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>0.094952647</v>
+        <v>0.038520704</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>0.09523756</v>
+        <v>0.038608653</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B24">
-        <v>0.096793249</v>
+        <v>0.036812626</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B25">
-        <v>0.097534458</v>
+        <v>0.035995053</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>0.099587879</v>
+        <v>0.039352217</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B27">
-        <v>0.100988122</v>
+        <v>0.036237016</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>0.101721571</v>
+        <v>0.039389467</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29">
-        <v>0.103807334</v>
+        <v>0.036358876</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B30">
-        <v>0.103401878</v>
+        <v>0.03672961</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>0.055725912</v>
+        <v>0.027526085</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>0.079140843</v>
+        <v>0.033266055</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B33">
-        <v>0.090835275</v>
+        <v>0.030367179</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>0.0917542</v>
+        <v>0.03530821</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B35">
-        <v>0.090023267</v>
+        <v>0.038402432</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B36">
-        <v>0.094497625</v>
+        <v>0.038193003</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B37">
-        <v>0.09505084</v>
+        <v>0.041805036</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B38">
-        <v>0.100662611</v>
+        <v>0.04797308</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B39">
-        <v>0.107754126</v>
+        <v>0.050549105</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B40">
-        <v>0.108813652</v>
+        <v>0.054241824</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B41">
-        <v>0.112644967</v>
+        <v>0.054692019</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B42">
-        <v>0.111859063</v>
+        <v>0.053147375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B43">
-        <v>0.117385718</v>
+        <v>0.041224534</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B44">
-        <v>0.129462114</v>
+        <v>0.047671258</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B45">
-        <v>0.131035289</v>
+        <v>0.055346255</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B46">
-        <v>0.131067487</v>
+        <v>0.052104236</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B47">
-        <v>0.132483732</v>
+        <v>0.055556281</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B48">
-        <v>0.146726631</v>
+        <v>0.053006782</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B49">
-        <v>0.150735142</v>
+        <v>0.055729972</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B50">
-        <v>0.151176512</v>
+        <v>0.051972068</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B51">
-        <v>0.152247409</v>
+        <v>0.052120135</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B52">
-        <v>0.152362311</v>
+        <v>0.055214151</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B53">
-        <v>0.151285354</v>
+        <v>0.055946422</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B54">
-        <v>0.151414743</v>
+        <v>0.061130872</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B55">
-        <v>0.155023994</v>
+        <v>0.057927207</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B56">
-        <v>0.154286342</v>
+        <v>0.059066338</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B57">
-        <v>0.157394463</v>
+        <v>0.059135688</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B58">
-        <v>0.157196172</v>
+        <v>0.058637837</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B59">
-        <v>0.159245777</v>
+        <v>0.058835125</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>0.158943761</v>
+        <v>0.056488408</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B61">
-        <v>0.1598626</v>
+        <v>0.033810076</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B62">
-        <v>0.161819036</v>
+        <v>0.040669898</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B63">
-        <v>0.186014825</v>
+        <v>0.047207231</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B64">
-        <v>0.196555341</v>
+        <v>0.049028063</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B65">
-        <v>0.194869333</v>
+        <v>0.047120246</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B66">
-        <v>0.195601522</v>
+        <v>0.052711772</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B67">
-        <v>0.196048734</v>
+        <v>0.053549651</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B68">
-        <v>0.196196485</v>
+        <v>0.057562642</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B69">
-        <v>0.203700647</v>
+        <v>0.058176117</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B70">
-        <v>0.201541376</v>
+        <v>0.061147602</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B71">
-        <v>0.209557581</v>
+        <v>0.059817289</v>
       </c>
     </row>
     <row r="72">
@@ -891,295 +891,295 @@
         <v>33</v>
       </c>
       <c r="B72">
-        <v>0.209837677</v>
+        <v>0.062101419</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B73">
-        <v>0.217650708</v>
+        <v>0.062491823</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B74">
-        <v>0.222516405</v>
+        <v>0.063181253</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B75">
-        <v>0.227664197</v>
+        <v>0.057813978</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B76">
-        <v>0.227635736</v>
+        <v>0.065374993</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B77">
-        <v>0.235115171</v>
+        <v>0.066467631</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B78">
-        <v>0.239100966</v>
+        <v>0.066072983</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B79">
-        <v>0.242256677</v>
+        <v>0.064688547</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B80">
-        <v>0.243151221</v>
+        <v>0.067596783</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B81">
-        <v>0.255646851</v>
+        <v>0.065325686</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B82">
-        <v>0.258447627</v>
+        <v>0.054502282</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B83">
-        <v>0.259167412</v>
+        <v>0.066570898</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B84">
-        <v>0.259295241</v>
+        <v>0.067938056</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B85">
-        <v>0.260315582</v>
+        <v>0.055704265</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B86">
-        <v>0.258894036</v>
+        <v>0.066804814</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B87">
-        <v>0.255906174</v>
+        <v>0.067557608</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B88">
-        <v>0.26042099</v>
+        <v>0.068466078</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B89">
-        <v>0.260105777</v>
+        <v>0.070158096</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B90">
-        <v>0.258385549</v>
+        <v>0.067198394</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B91">
-        <v>0.263093234</v>
+        <v>0.068815719</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B92">
-        <v>0.258578007</v>
+        <v>0.073029841</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B93">
-        <v>0.263886682</v>
+        <v>0.060279152</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B94">
-        <v>0.260761762</v>
+        <v>0.072944631</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B95">
-        <v>0.262237833</v>
+        <v>0.075613699</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B96">
-        <v>0.257714547</v>
+        <v>0.073551975</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B97">
-        <v>0.257711819</v>
+        <v>0.075767434</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B98">
-        <v>0.263716378</v>
+        <v>0.076872671</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B99">
-        <v>0.264606393</v>
+        <v>0.062547886</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B100">
-        <v>0.265317335</v>
+        <v>0.068755507</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B101">
-        <v>0.081649763</v>
+        <v>0.042695902</v>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B102">
-        <v>0.107419064</v>
+        <v>0.055401618</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B103">
-        <v>0.109129252</v>
+        <v>0.0593382</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B104">
-        <v>0.126432831</v>
+        <v>0.057510612</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B105">
-        <v>0.127552879</v>
+        <v>0.06003737</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B106">
-        <v>0.147646057</v>
+        <v>0.060187574</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B107">
-        <v>0.151615046</v>
+        <v>0.061602754</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B108">
-        <v>0.154714915</v>
+        <v>0.058232955</v>
       </c>
     </row>
     <row r="109">
@@ -1187,47 +1187,47 @@
         <v>45</v>
       </c>
       <c r="B109">
-        <v>0.155763298</v>
+        <v>0.065527871</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B110">
-        <v>0.156747269</v>
+        <v>0.06561295</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B111">
-        <v>0.157374571</v>
+        <v>0.065666071</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B112">
-        <v>0.165145037</v>
+        <v>0.067868125</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B113">
-        <v>0.166330789</v>
+        <v>0.065132677</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B114">
-        <v>0.16491366</v>
+        <v>0.067025219</v>
       </c>
     </row>
     <row r="115">
@@ -1235,591 +1235,591 @@
         <v>19</v>
       </c>
       <c r="B115">
-        <v>0.170303407</v>
+        <v>0.065598023</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B116">
-        <v>0.171451071</v>
+        <v>0.06833002</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B117">
-        <v>0.184077545</v>
+        <v>0.068948297</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B118">
-        <v>0.183167686</v>
+        <v>0.069050958</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B119">
-        <v>0.187068862</v>
+        <v>0.068165444</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B120">
-        <v>0.22163369</v>
+        <v>0.069669286</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B121">
-        <v>0.230699825</v>
+        <v>0.065015732</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B122">
-        <v>0.234920873</v>
+        <v>0.06904111</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B123">
-        <v>0.236164595</v>
+        <v>0.065589332</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B124">
-        <v>0.235485372</v>
+        <v>0.067268803</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B125">
-        <v>0.242337107</v>
+        <v>0.069320161</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B126">
-        <v>0.240301486</v>
+        <v>0.06904594</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B127">
-        <v>0.246158147</v>
+        <v>0.069479839</v>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B128">
-        <v>0.245611733</v>
+        <v>0.068219486</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B129">
-        <v>0.246688633</v>
+        <v>0.069986571</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B130">
-        <v>0.252140271</v>
+        <v>0.071383114</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B131">
-        <v>0.251957595</v>
+        <v>0.069685971</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B132">
-        <v>0.250128343</v>
+        <v>0.071246697</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B133">
-        <v>0.249672472</v>
+        <v>0.068641075</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B134">
-        <v>0.250012362</v>
+        <v>0.072745295</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B135">
-        <v>0.254266244</v>
+        <v>0.072970807</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B136">
-        <v>0.253985911</v>
+        <v>0.069230056</v>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B137">
-        <v>0.252957996</v>
+        <v>0.069534683</v>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B138">
-        <v>0.255509554</v>
+        <v>0.074250036</v>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B139">
-        <v>0.255239759</v>
+        <v>0.069991255</v>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B140">
-        <v>0.255107379</v>
+        <v>0.071580006</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B141">
-        <v>0.254398851</v>
+        <v>0.070401256</v>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B142">
-        <v>0.256372814</v>
+        <v>0.071947207</v>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B143">
-        <v>0.252238917</v>
+        <v>0.071975873</v>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B144">
-        <v>0.257861042</v>
+        <v>0.069994748</v>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B145">
-        <v>0.25368055</v>
+        <v>0.074724063</v>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B146">
-        <v>0.255809325</v>
+        <v>0.072384617</v>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B147">
-        <v>0.251143223</v>
+        <v>0.070914994</v>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B148">
-        <v>0.258733465</v>
+        <v>0.072629338</v>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B149">
-        <v>0.260044644</v>
+        <v>0.070507213</v>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B150">
-        <v>0.26075392</v>
+        <v>0.073851351</v>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B151">
-        <v>0.10275533</v>
+        <v>0.031358997</v>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B152">
-        <v>0.119138472</v>
+        <v>0.038435597</v>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B153">
-        <v>0.134458203</v>
+        <v>0.048545166</v>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B154">
-        <v>0.132489444</v>
+        <v>0.051783699</v>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B155">
-        <v>0.134067088</v>
+        <v>0.044581997</v>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B156">
-        <v>0.136277271</v>
+        <v>0.050424732</v>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B157">
-        <v>0.151522366</v>
+        <v>0.045167403</v>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B158">
-        <v>0.176002146</v>
+        <v>0.05096141</v>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B159">
-        <v>0.179019681</v>
+        <v>0.058315778</v>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B160">
-        <v>0.180436683</v>
+        <v>0.057657953</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B161">
-        <v>0.183846928</v>
+        <v>0.057357296</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B162">
-        <v>0.186363529</v>
+        <v>0.052188002</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B163">
-        <v>0.185612386</v>
+        <v>0.061573477</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B164">
-        <v>0.191547321</v>
+        <v>0.057021951</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B165">
-        <v>0.191276462</v>
+        <v>0.065405584</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B166">
-        <v>0.190479857</v>
+        <v>0.065377782</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B167">
-        <v>0.192967139</v>
+        <v>0.067339732</v>
       </c>
     </row>
     <row r="168">
       <c r="A168">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B168">
-        <v>0.192580912</v>
+        <v>0.069835123</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B169">
-        <v>0.192139762</v>
+        <v>0.068540298</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B170">
-        <v>0.193551954</v>
+        <v>0.067407731</v>
       </c>
     </row>
     <row r="171">
       <c r="A171">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B171">
-        <v>0.193798124</v>
+        <v>0.070260315</v>
       </c>
     </row>
     <row r="172">
       <c r="A172">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B172">
-        <v>0.193768529</v>
+        <v>0.066481033</v>
       </c>
     </row>
     <row r="173">
       <c r="A173">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B173">
-        <v>0.199672367</v>
+        <v>0.062737741</v>
       </c>
     </row>
     <row r="174">
       <c r="A174">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B174">
-        <v>0.200842077</v>
+        <v>0.065007292</v>
       </c>
     </row>
     <row r="175">
       <c r="A175">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B175">
-        <v>0.200953382</v>
+        <v>0.067646621</v>
       </c>
     </row>
     <row r="176">
       <c r="A176">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B176">
-        <v>0.208456319</v>
+        <v>0.070369688</v>
       </c>
     </row>
     <row r="177">
       <c r="A177">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B177">
-        <v>0.216404551</v>
+        <v>0.067930976</v>
       </c>
     </row>
     <row r="178">
       <c r="A178">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B178">
-        <v>0.224669604</v>
+        <v>0.067849734</v>
       </c>
     </row>
     <row r="179">
       <c r="A179">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B179">
-        <v>0.223187328</v>
+        <v>0.067382595</v>
       </c>
     </row>
     <row r="180">
       <c r="A180">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B180">
-        <v>0.225274389</v>
+        <v>0.06791901</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B181">
-        <v>0.235290104</v>
+        <v>0.070193223</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B182">
-        <v>0.234322921</v>
+        <v>0.071217813</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B183">
-        <v>0.237192722</v>
+        <v>0.072073004</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B184">
-        <v>0.253686791</v>
+        <v>0.071677722</v>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B185">
-        <v>0.254138221</v>
+        <v>0.077020077</v>
       </c>
     </row>
     <row r="186">
       <c r="A186">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B186">
-        <v>0.257371038</v>
+        <v>0.076414554</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B187">
-        <v>0.25775672</v>
+        <v>0.077677258</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B188">
-        <v>0.258994597</v>
+        <v>0.077473392</v>
       </c>
     </row>
     <row r="189">
@@ -1827,575 +1827,575 @@
         <v>22</v>
       </c>
       <c r="B189">
-        <v>0.258145927</v>
+        <v>0.075373329</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="B190">
-        <v>0.260358552</v>
+        <v>0.078953315</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B191">
-        <v>0.25789606</v>
+        <v>0.082549972</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B192">
-        <v>0.259879085</v>
+        <v>0.077943539</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="B193">
-        <v>0.259189622</v>
+        <v>0.076265518</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B194">
-        <v>0.259766053</v>
+        <v>0.084552977</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B195">
-        <v>0.260156462</v>
+        <v>0.077115084</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B196">
-        <v>0.260117914</v>
+        <v>0.081724888</v>
       </c>
     </row>
     <row r="197">
       <c r="A197">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B197">
-        <v>0.259208036</v>
+        <v>0.082210168</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B198">
-        <v>0.259751794</v>
+        <v>0.083315113</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B199">
-        <v>0.260525598</v>
+        <v>0.081628884</v>
       </c>
     </row>
     <row r="200">
       <c r="A200">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B200">
-        <v>0.2633431</v>
+        <v>0.082443105</v>
       </c>
     </row>
     <row r="201">
       <c r="A201">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B201">
-        <v>0.261315392</v>
+        <v>0.084787232</v>
       </c>
     </row>
     <row r="202">
       <c r="A202">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B202">
-        <v>0.260796965</v>
+        <v>0.082924787</v>
       </c>
     </row>
     <row r="203">
       <c r="A203">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B203">
-        <v>0.265178879</v>
+        <v>0.082855253</v>
       </c>
     </row>
     <row r="204">
       <c r="A204">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B204">
-        <v>0.264890999</v>
+        <v>0.083478322</v>
       </c>
     </row>
     <row r="205">
       <c r="A205">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B205">
-        <v>0.267530829</v>
+        <v>0.087471582</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B206">
-        <v>0.266534977</v>
+        <v>0.087066359</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B207">
-        <v>0.265834628</v>
+        <v>0.085331231</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B208">
-        <v>0.267701496</v>
+        <v>0.085491067</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="B209">
-        <v>0.268670145</v>
+        <v>0.083668786</v>
       </c>
     </row>
     <row r="210">
       <c r="A210">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B210">
-        <v>0.268160735</v>
+        <v>0.086800859</v>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B211">
-        <v>0.098053802</v>
+        <v>0.039978165</v>
       </c>
     </row>
     <row r="212">
       <c r="A212">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B212">
-        <v>0.125855421</v>
+        <v>0.042103166</v>
       </c>
     </row>
     <row r="213">
       <c r="A213">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B213">
-        <v>0.130087186</v>
+        <v>0.045165661</v>
       </c>
     </row>
     <row r="214">
       <c r="A214">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B214">
-        <v>0.132769264</v>
+        <v>0.045658147</v>
       </c>
     </row>
     <row r="215">
       <c r="A215">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B215">
-        <v>0.135157691</v>
+        <v>0.052734089</v>
       </c>
     </row>
     <row r="216">
       <c r="A216">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B216">
-        <v>0.141222236</v>
+        <v>0.054090364</v>
       </c>
     </row>
     <row r="217">
       <c r="A217">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B217">
-        <v>0.156072255</v>
+        <v>0.055318605</v>
       </c>
     </row>
     <row r="218">
       <c r="A218">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B218">
-        <v>0.160360236</v>
+        <v>0.056798178</v>
       </c>
     </row>
     <row r="219">
       <c r="A219">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B219">
-        <v>0.169616947</v>
+        <v>0.061258429</v>
       </c>
     </row>
     <row r="220">
       <c r="A220">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B220">
-        <v>0.172132321</v>
+        <v>0.059854504</v>
       </c>
     </row>
     <row r="221">
       <c r="A221">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B221">
-        <v>0.185851072</v>
+        <v>0.06188213</v>
       </c>
     </row>
     <row r="222">
       <c r="A222">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B222">
-        <v>0.199334212</v>
+        <v>0.065212913</v>
       </c>
     </row>
     <row r="223">
       <c r="A223">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B223">
-        <v>0.208970357</v>
+        <v>0.067125908</v>
       </c>
     </row>
     <row r="224">
       <c r="A224">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B224">
-        <v>0.209561278</v>
+        <v>0.069061857</v>
       </c>
     </row>
     <row r="225">
       <c r="A225">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B225">
-        <v>0.207809325</v>
+        <v>0.07061962</v>
       </c>
     </row>
     <row r="226">
       <c r="A226">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B226">
-        <v>0.221589757</v>
+        <v>0.070276375</v>
       </c>
     </row>
     <row r="227">
       <c r="A227">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B227">
-        <v>0.221374159</v>
+        <v>0.069685645</v>
       </c>
     </row>
     <row r="228">
       <c r="A228">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B228">
-        <v>0.220863458</v>
+        <v>0.068409859</v>
       </c>
     </row>
     <row r="229">
       <c r="A229">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B229">
-        <v>0.22590966</v>
+        <v>0.072544355</v>
       </c>
     </row>
     <row r="230">
       <c r="A230">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B230">
-        <v>0.224778559</v>
+        <v>0.068713122</v>
       </c>
     </row>
     <row r="231">
       <c r="A231">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B231">
-        <v>0.235392453</v>
+        <v>0.068622501</v>
       </c>
     </row>
     <row r="232">
       <c r="A232">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B232">
-        <v>0.237675731</v>
+        <v>0.074125916</v>
       </c>
     </row>
     <row r="233">
       <c r="A233">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B233">
-        <v>0.238670879</v>
+        <v>0.076258497</v>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B234">
-        <v>0.248358827</v>
+        <v>0.077470123</v>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B235">
-        <v>0.264386856</v>
+        <v>0.079683068</v>
       </c>
     </row>
     <row r="236">
       <c r="A236">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B236">
-        <v>0.265105889</v>
+        <v>0.077891748</v>
       </c>
     </row>
     <row r="237">
       <c r="A237">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B237">
-        <v>0.264055276</v>
+        <v>0.079456192</v>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="B238">
-        <v>0.266686087</v>
+        <v>0.0800524</v>
       </c>
     </row>
     <row r="239">
       <c r="A239">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B239">
-        <v>0.26590226</v>
+        <v>0.079275173</v>
       </c>
     </row>
     <row r="240">
       <c r="A240">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B240">
-        <v>0.269597561</v>
+        <v>0.078822175</v>
       </c>
     </row>
     <row r="241">
       <c r="A241">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B241">
-        <v>0.270012632</v>
+        <v>0.080463815</v>
       </c>
     </row>
     <row r="242">
       <c r="A242">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B242">
-        <v>0.270553277</v>
+        <v>0.078197455</v>
       </c>
     </row>
     <row r="243">
       <c r="A243">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B243">
-        <v>0.272008284</v>
+        <v>0.079989884</v>
       </c>
     </row>
     <row r="244">
       <c r="A244">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B244">
-        <v>0.275765832</v>
+        <v>0.078982628</v>
       </c>
     </row>
     <row r="245">
       <c r="A245">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B245">
-        <v>0.279991452</v>
+        <v>0.080486945</v>
       </c>
     </row>
     <row r="246">
       <c r="A246">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B246">
-        <v>0.277136265</v>
+        <v>0.083562338</v>
       </c>
     </row>
     <row r="247">
       <c r="A247">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B247">
-        <v>0.281395993</v>
+        <v>0.078044821</v>
       </c>
     </row>
     <row r="248">
       <c r="A248">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B248">
-        <v>0.279083395</v>
+        <v>0.08426845</v>
       </c>
     </row>
     <row r="249">
       <c r="A249">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B249">
-        <v>0.279094641</v>
+        <v>0.078022306</v>
       </c>
     </row>
     <row r="250">
       <c r="A250">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B250">
-        <v>0.281170973</v>
+        <v>0.077018871</v>
       </c>
     </row>
     <row r="251">
       <c r="A251">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B251">
-        <v>0.280874323</v>
+        <v>0.078145935</v>
       </c>
     </row>
     <row r="252">
       <c r="A252">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B252">
-        <v>0.281657999</v>
+        <v>0.077976482</v>
       </c>
     </row>
     <row r="253">
       <c r="A253">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B253">
-        <v>0.281357698</v>
+        <v>0.077697463</v>
       </c>
     </row>
     <row r="254">
       <c r="A254">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B254">
-        <v>0.282785623</v>
+        <v>0.076834829</v>
       </c>
     </row>
     <row r="255">
       <c r="A255">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B255">
-        <v>0.282998526</v>
+        <v>0.077066824</v>
       </c>
     </row>
     <row r="256">
       <c r="A256">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B256">
-        <v>0.284995363</v>
+        <v>0.083948408</v>
       </c>
     </row>
     <row r="257">
       <c r="A257">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B257">
-        <v>0.286717109</v>
+        <v>0.077165617</v>
       </c>
     </row>
     <row r="258">
       <c r="A258">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B258">
-        <v>0.287102004</v>
+        <v>0.079301581</v>
       </c>
     </row>
     <row r="259">
       <c r="A259">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B259">
-        <v>0.290964085</v>
+        <v>0.086839459</v>
       </c>
     </row>
     <row r="260">
       <c r="A260">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B260">
-        <v>0.294795661</v>
+        <v>0.086002542</v>
       </c>
     </row>
     <row r="261">
@@ -2403,127 +2403,127 @@
         <v>63</v>
       </c>
       <c r="B261">
-        <v>0.295752201</v>
+        <v>0.085423932</v>
       </c>
     </row>
     <row r="262">
       <c r="A262">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B262">
-        <v>0.295083489</v>
+        <v>0.089985151</v>
       </c>
     </row>
     <row r="263">
       <c r="A263">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B263">
-        <v>0.293997978</v>
+        <v>0.087603987</v>
       </c>
     </row>
     <row r="264">
       <c r="A264">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B264">
-        <v>0.293325978</v>
+        <v>0.087388405</v>
       </c>
     </row>
     <row r="265">
       <c r="A265">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B265">
-        <v>0.294126903</v>
+        <v>0.090179638</v>
       </c>
     </row>
     <row r="266">
       <c r="A266">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B266">
-        <v>0.298660961</v>
+        <v>0.088745223</v>
       </c>
     </row>
     <row r="267">
       <c r="A267">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B267">
-        <v>0.299578491</v>
+        <v>0.090154798</v>
       </c>
     </row>
     <row r="268">
       <c r="A268">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B268">
-        <v>0.305778722</v>
+        <v>0.08917516</v>
       </c>
     </row>
     <row r="269">
       <c r="A269">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B269">
-        <v>0.307608813</v>
+        <v>0.088951367</v>
       </c>
     </row>
     <row r="270">
       <c r="A270">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B270">
-        <v>0.311379002</v>
+        <v>0.090679536</v>
       </c>
     </row>
     <row r="271">
       <c r="A271">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B271">
-        <v>0.306949776</v>
+        <v>0.090720135</v>
       </c>
     </row>
     <row r="272">
       <c r="A272">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B272">
-        <v>0.312919621</v>
+        <v>0.090133978</v>
       </c>
     </row>
     <row r="273">
       <c r="A273">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B273">
-        <v>0.314241969</v>
+        <v>0.090794897</v>
       </c>
     </row>
     <row r="274">
       <c r="A274">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B274">
-        <v>0.314706152</v>
+        <v>0.090968343</v>
       </c>
     </row>
     <row r="275">
       <c r="A275">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B275">
-        <v>0.316826837</v>
+        <v>0.087893379</v>
       </c>
     </row>
     <row r="276">
       <c r="A276">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B276">
-        <v>0.317544321</v>
+        <v>0.088904431</v>
       </c>
     </row>
     <row r="277">
@@ -2531,807 +2531,807 @@
         <v>6</v>
       </c>
       <c r="B277">
-        <v>0.315793148</v>
+        <v>0.090430037</v>
       </c>
     </row>
     <row r="278">
       <c r="A278">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B278">
-        <v>0.3211087</v>
+        <v>0.089262472</v>
       </c>
     </row>
     <row r="279">
       <c r="A279">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B279">
-        <v>0.31948169</v>
+        <v>0.088756981</v>
       </c>
     </row>
     <row r="280">
       <c r="A280">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B280">
-        <v>0.320565899</v>
+        <v>0.090771261</v>
       </c>
     </row>
     <row r="281">
       <c r="A281">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="B281">
-        <v>0.12221927</v>
+        <v>0.044992362</v>
       </c>
     </row>
     <row r="282">
       <c r="A282">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B282">
-        <v>0.143774119</v>
+        <v>0.047628864</v>
       </c>
     </row>
     <row r="283">
       <c r="A283">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B283">
-        <v>0.149981463</v>
+        <v>0.048267048</v>
       </c>
     </row>
     <row r="284">
       <c r="A284">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B284">
-        <v>0.162363201</v>
+        <v>0.061270557</v>
       </c>
     </row>
     <row r="285">
       <c r="A285">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B285">
-        <v>0.170026629</v>
+        <v>0.060037707</v>
       </c>
     </row>
     <row r="286">
       <c r="A286">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B286">
-        <v>0.167681809</v>
+        <v>0.067283279</v>
       </c>
     </row>
     <row r="287">
       <c r="A287">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B287">
-        <v>0.166928556</v>
+        <v>0.073798214</v>
       </c>
     </row>
     <row r="288">
       <c r="A288">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B288">
-        <v>0.16758718</v>
+        <v>0.072583296</v>
       </c>
     </row>
     <row r="289">
       <c r="A289">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B289">
-        <v>0.167838596</v>
+        <v>0.073622722</v>
       </c>
     </row>
     <row r="290">
       <c r="A290">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B290">
-        <v>0.178550404</v>
+        <v>0.065030716</v>
       </c>
     </row>
     <row r="291">
       <c r="A291">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="B291">
-        <v>0.178060642</v>
+        <v>0.075253905</v>
       </c>
     </row>
     <row r="292">
       <c r="A292">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B292">
-        <v>0.179384781</v>
+        <v>0.074070103</v>
       </c>
     </row>
     <row r="293">
       <c r="A293">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B293">
-        <v>0.182313995</v>
+        <v>0.073586599</v>
       </c>
     </row>
     <row r="294">
       <c r="A294">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B294">
-        <v>0.175417817</v>
+        <v>0.073799878</v>
       </c>
     </row>
     <row r="295">
       <c r="A295">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B295">
-        <v>0.18354213</v>
+        <v>0.076707492</v>
       </c>
     </row>
     <row r="296">
       <c r="A296">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B296">
-        <v>0.191362293</v>
+        <v>0.07612485</v>
       </c>
     </row>
     <row r="297">
       <c r="A297">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B297">
-        <v>0.211067245</v>
+        <v>0.071791315</v>
       </c>
     </row>
     <row r="298">
       <c r="A298">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B298">
-        <v>0.211873667</v>
+        <v>0.07074574</v>
       </c>
     </row>
     <row r="299">
       <c r="A299">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B299">
-        <v>0.215195769</v>
+        <v>0.076179128</v>
       </c>
     </row>
     <row r="300">
       <c r="A300">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B300">
-        <v>0.216841659</v>
+        <v>0.07154713</v>
       </c>
     </row>
     <row r="301">
       <c r="A301">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B301">
-        <v>0.214257048</v>
+        <v>0.079417507</v>
       </c>
     </row>
     <row r="302">
       <c r="A302">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="B302">
-        <v>0.218355528</v>
+        <v>0.074188335</v>
       </c>
     </row>
     <row r="303">
       <c r="A303">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B303">
-        <v>0.215370408</v>
+        <v>0.071772863</v>
       </c>
     </row>
     <row r="304">
       <c r="A304">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B304">
-        <v>0.216801114</v>
+        <v>0.079012727</v>
       </c>
     </row>
     <row r="305">
       <c r="A305">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B305">
-        <v>0.218943659</v>
+        <v>0.072797613</v>
       </c>
     </row>
     <row r="306">
       <c r="A306">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B306">
-        <v>0.231913591</v>
+        <v>0.071523066</v>
       </c>
     </row>
     <row r="307">
       <c r="A307">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B307">
-        <v>0.232126111</v>
+        <v>0.072125381</v>
       </c>
     </row>
     <row r="308">
       <c r="A308">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B308">
-        <v>0.234879805</v>
+        <v>0.078010898</v>
       </c>
     </row>
     <row r="309">
       <c r="A309">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B309">
-        <v>0.236153717</v>
+        <v>0.076929786</v>
       </c>
     </row>
     <row r="310">
       <c r="A310">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B310">
-        <v>0.243650489</v>
+        <v>0.078789033</v>
       </c>
     </row>
     <row r="311">
       <c r="A311">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="B311">
-        <v>0.247463208</v>
+        <v>0.076656388</v>
       </c>
     </row>
     <row r="312">
       <c r="A312">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B312">
-        <v>0.245327177</v>
+        <v>0.079650606</v>
       </c>
     </row>
     <row r="313">
       <c r="A313">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="B313">
-        <v>0.244041684</v>
+        <v>0.080037334</v>
       </c>
     </row>
     <row r="314">
       <c r="A314">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B314">
-        <v>0.244203139</v>
+        <v>0.078362459</v>
       </c>
     </row>
     <row r="315">
       <c r="A315">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B315">
-        <v>0.251522709</v>
+        <v>0.084028956</v>
       </c>
     </row>
     <row r="316">
       <c r="A316">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B316">
-        <v>0.251277682</v>
+        <v>0.084148037</v>
       </c>
     </row>
     <row r="317">
       <c r="A317">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B317">
-        <v>0.248534664</v>
+        <v>0.086041094</v>
       </c>
     </row>
     <row r="318">
       <c r="A318">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B318">
-        <v>0.249520461</v>
+        <v>0.081475462</v>
       </c>
     </row>
     <row r="319">
       <c r="A319">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B319">
-        <v>0.250844961</v>
+        <v>0.088243441</v>
       </c>
     </row>
     <row r="320">
       <c r="A320">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B320">
-        <v>0.25012224</v>
+        <v>0.083562004</v>
       </c>
     </row>
     <row r="321">
       <c r="A321">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="B321">
-        <v>0.246483878</v>
+        <v>0.089479963</v>
       </c>
     </row>
     <row r="322">
       <c r="A322">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B322">
-        <v>0.275802432</v>
+        <v>0.086098443</v>
       </c>
     </row>
     <row r="323">
       <c r="A323">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B323">
-        <v>0.284593602</v>
+        <v>0.081912982</v>
       </c>
     </row>
     <row r="324">
       <c r="A324">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B324">
-        <v>0.284301326</v>
+        <v>0.086727528</v>
       </c>
     </row>
     <row r="325">
       <c r="A325">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B325">
-        <v>0.28922184</v>
+        <v>0.090718575</v>
       </c>
     </row>
     <row r="326">
       <c r="A326">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B326">
-        <v>0.286468677</v>
+        <v>0.083486846</v>
       </c>
     </row>
     <row r="327">
       <c r="A327">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="B327">
-        <v>0.297637648</v>
+        <v>0.083273596</v>
       </c>
     </row>
     <row r="328">
       <c r="A328">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B328">
-        <v>0.301509982</v>
+        <v>0.090233141</v>
       </c>
     </row>
     <row r="329">
       <c r="A329">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B329">
-        <v>0.303635434</v>
+        <v>0.08614671</v>
       </c>
     </row>
     <row r="330">
       <c r="A330">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="B330">
-        <v>0.310994366</v>
+        <v>0.083204129</v>
       </c>
     </row>
     <row r="331">
       <c r="A331">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B331">
-        <v>0.309226208</v>
+        <v>0.085389038</v>
       </c>
     </row>
     <row r="332">
       <c r="A332">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B332">
-        <v>0.305844788</v>
+        <v>0.088884117</v>
       </c>
     </row>
     <row r="333">
       <c r="A333">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B333">
-        <v>0.30870498</v>
+        <v>0.084754429</v>
       </c>
     </row>
     <row r="334">
       <c r="A334">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B334">
-        <v>0.307354809</v>
+        <v>0.091229364</v>
       </c>
     </row>
     <row r="335">
       <c r="A335">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B335">
-        <v>0.312809603</v>
+        <v>0.088064758</v>
       </c>
     </row>
     <row r="336">
       <c r="A336">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B336">
-        <v>0.31170856</v>
+        <v>0.086573916</v>
       </c>
     </row>
     <row r="337">
       <c r="A337">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="B337">
-        <v>0.313240319</v>
+        <v>0.082508475</v>
       </c>
     </row>
     <row r="338">
       <c r="A338">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="B338">
-        <v>0.314558907</v>
+        <v>0.082691358</v>
       </c>
     </row>
     <row r="339">
       <c r="A339">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B339">
-        <v>0.308319148</v>
+        <v>0.093482806</v>
       </c>
     </row>
     <row r="340">
       <c r="A340">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B340">
-        <v>0.315231866</v>
+        <v>0.083655818</v>
       </c>
     </row>
     <row r="341">
       <c r="A341">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B341">
-        <v>0.321466129</v>
+        <v>0.087056664</v>
       </c>
     </row>
     <row r="342">
       <c r="A342">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B342">
-        <v>0.317058761</v>
+        <v>0.090439733</v>
       </c>
     </row>
     <row r="343">
       <c r="A343">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B343">
-        <v>0.317695141</v>
+        <v>0.093097958</v>
       </c>
     </row>
     <row r="344">
       <c r="A344">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B344">
-        <v>0.317412314</v>
+        <v>0.088991673</v>
       </c>
     </row>
     <row r="345">
       <c r="A345">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B345">
-        <v>0.318787026</v>
+        <v>0.095495327</v>
       </c>
     </row>
     <row r="346">
       <c r="A346">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B346">
-        <v>0.314880656</v>
+        <v>0.086333079</v>
       </c>
     </row>
     <row r="347">
       <c r="A347">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B347">
-        <v>0.321466026</v>
+        <v>0.091607561</v>
       </c>
     </row>
     <row r="348">
       <c r="A348">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B348">
-        <v>0.319957637</v>
+        <v>0.092856606</v>
       </c>
     </row>
     <row r="349">
       <c r="A349">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B349">
-        <v>0.318828273</v>
+        <v>0.090486057</v>
       </c>
     </row>
     <row r="350">
       <c r="A350">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B350">
-        <v>0.318629547</v>
+        <v>0.087089059</v>
       </c>
     </row>
     <row r="351">
       <c r="A351">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="B351">
-        <v>0.315949843</v>
+        <v>0.088657405</v>
       </c>
     </row>
     <row r="352">
       <c r="A352">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B352">
-        <v>0.322571376</v>
+        <v>0.089218202</v>
       </c>
     </row>
     <row r="353">
       <c r="A353">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="B353">
-        <v>0.319364933</v>
+        <v>0.09085611</v>
       </c>
     </row>
     <row r="354">
       <c r="A354">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B354">
-        <v>0.319575045</v>
+        <v>0.093753343</v>
       </c>
     </row>
     <row r="355">
       <c r="A355">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B355">
-        <v>0.32632485</v>
+        <v>0.094056371</v>
       </c>
     </row>
     <row r="356">
       <c r="A356">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B356">
-        <v>0.323501453</v>
+        <v>0.090396287</v>
       </c>
     </row>
     <row r="357">
       <c r="A357">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B357">
-        <v>0.327407051</v>
+        <v>0.09064138</v>
       </c>
     </row>
     <row r="358">
       <c r="A358">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B358">
-        <v>0.327850158</v>
+        <v>0.08807389</v>
       </c>
     </row>
     <row r="359">
       <c r="A359">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B359">
-        <v>0.327314838</v>
+        <v>0.088940253</v>
       </c>
     </row>
     <row r="360">
       <c r="A360">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B360">
-        <v>0.327445432</v>
+        <v>0.090437656</v>
       </c>
     </row>
     <row r="361">
       <c r="A361">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B361">
-        <v>0.117204645</v>
+        <v>0.060055635</v>
       </c>
     </row>
     <row r="362">
       <c r="A362">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B362">
-        <v>0.125465068</v>
+        <v>0.061881488</v>
       </c>
     </row>
     <row r="363">
       <c r="A363">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B363">
-        <v>0.132363119</v>
+        <v>0.067316978</v>
       </c>
     </row>
     <row r="364">
       <c r="A364">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="B364">
-        <v>0.133401358</v>
+        <v>0.081395405</v>
       </c>
     </row>
     <row r="365">
       <c r="A365">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B365">
-        <v>0.136601004</v>
+        <v>0.081377172</v>
       </c>
     </row>
     <row r="366">
       <c r="A366">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B366">
-        <v>0.140475073</v>
+        <v>0.085170074</v>
       </c>
     </row>
     <row r="367">
       <c r="A367">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B367">
-        <v>0.152373112</v>
+        <v>0.084968131</v>
       </c>
     </row>
     <row r="368">
       <c r="A368">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B368">
-        <v>0.146184445</v>
+        <v>0.085848606</v>
       </c>
     </row>
     <row r="369">
       <c r="A369">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B369">
-        <v>0.1732365</v>
+        <v>0.083866888</v>
       </c>
     </row>
     <row r="370">
       <c r="A370">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B370">
-        <v>0.180678916</v>
+        <v>0.085096283</v>
       </c>
     </row>
     <row r="371">
       <c r="A371">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B371">
-        <v>0.190084582</v>
+        <v>0.083955333</v>
       </c>
     </row>
     <row r="372">
       <c r="A372">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B372">
-        <v>0.191575085</v>
+        <v>0.086473781</v>
       </c>
     </row>
     <row r="373">
       <c r="A373">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="B373">
-        <v>0.195537639</v>
+        <v>0.08660982</v>
       </c>
     </row>
     <row r="374">
       <c r="A374">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B374">
-        <v>0.19867102</v>
+        <v>0.086652175</v>
       </c>
     </row>
     <row r="375">
       <c r="A375">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B375">
-        <v>0.204070376</v>
+        <v>0.085856772</v>
       </c>
     </row>
     <row r="376">
       <c r="A376">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="B376">
-        <v>0.205610934</v>
+        <v>0.084556606</v>
       </c>
     </row>
     <row r="377">
       <c r="A377">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B377">
-        <v>0.223901235</v>
+        <v>0.084734034</v>
       </c>
     </row>
     <row r="378">
@@ -3339,583 +3339,583 @@
         <v>47</v>
       </c>
       <c r="B378">
-        <v>0.21320777</v>
+        <v>0.087412329</v>
       </c>
     </row>
     <row r="379">
       <c r="A379">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B379">
-        <v>0.223069759</v>
+        <v>0.087122011</v>
       </c>
     </row>
     <row r="380">
       <c r="A380">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B380">
-        <v>0.229919016</v>
+        <v>0.087724677</v>
       </c>
     </row>
     <row r="381">
       <c r="A381">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B381">
-        <v>0.229821287</v>
+        <v>0.085382046</v>
       </c>
     </row>
     <row r="382">
       <c r="A382">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B382">
-        <v>0.233180525</v>
+        <v>0.083426503</v>
       </c>
     </row>
     <row r="383">
       <c r="A383">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B383">
-        <v>0.237174697</v>
+        <v>0.082914651</v>
       </c>
     </row>
     <row r="384">
       <c r="A384">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B384">
-        <v>0.235985876</v>
+        <v>0.08617844</v>
       </c>
     </row>
     <row r="385">
       <c r="A385">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B385">
-        <v>0.237820763</v>
+        <v>0.088289998</v>
       </c>
     </row>
     <row r="386">
       <c r="A386">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B386">
-        <v>0.240499024</v>
+        <v>0.089124537</v>
       </c>
     </row>
     <row r="387">
       <c r="A387">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B387">
-        <v>0.250264317</v>
+        <v>0.090624536</v>
       </c>
     </row>
     <row r="388">
       <c r="A388">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B388">
-        <v>0.251103177</v>
+        <v>0.101075006</v>
       </c>
     </row>
     <row r="389">
       <c r="A389">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B389">
-        <v>0.253459987</v>
+        <v>0.100923481</v>
       </c>
     </row>
     <row r="390">
       <c r="A390">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B390">
-        <v>0.248533388</v>
+        <v>0.101721254</v>
       </c>
     </row>
     <row r="391">
       <c r="A391">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B391">
-        <v>0.255788044</v>
+        <v>0.100711558</v>
       </c>
     </row>
     <row r="392">
       <c r="A392">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B392">
-        <v>0.255085105</v>
+        <v>0.101925901</v>
       </c>
     </row>
     <row r="393">
       <c r="A393">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B393">
-        <v>0.259209061</v>
+        <v>0.102740723</v>
       </c>
     </row>
     <row r="394">
       <c r="A394">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B394">
-        <v>0.260832367</v>
+        <v>0.105134934</v>
       </c>
     </row>
     <row r="395">
       <c r="A395">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B395">
-        <v>0.264951626</v>
+        <v>0.105163051</v>
       </c>
     </row>
     <row r="396">
       <c r="A396">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B396">
-        <v>0.266861741</v>
+        <v>0.096174155</v>
       </c>
     </row>
     <row r="397">
       <c r="A397">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B397">
-        <v>0.275734562</v>
+        <v>0.104815455</v>
       </c>
     </row>
     <row r="398">
       <c r="A398">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B398">
-        <v>0.279498632</v>
+        <v>0.105586645</v>
       </c>
     </row>
     <row r="399">
       <c r="A399">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B399">
-        <v>0.280660709</v>
+        <v>0.104133114</v>
       </c>
     </row>
     <row r="400">
       <c r="A400">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="B400">
-        <v>0.281483118</v>
+        <v>0.105917123</v>
       </c>
     </row>
     <row r="401">
       <c r="A401">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B401">
-        <v>0.279710618</v>
+        <v>0.092645903</v>
       </c>
     </row>
     <row r="402">
       <c r="A402">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B402">
-        <v>0.276893385</v>
+        <v>0.104014298</v>
       </c>
     </row>
     <row r="403">
       <c r="A403">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B403">
-        <v>0.28745742</v>
+        <v>0.102981471</v>
       </c>
     </row>
     <row r="404">
       <c r="A404">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B404">
-        <v>0.284028825</v>
+        <v>0.103793464</v>
       </c>
     </row>
     <row r="405">
       <c r="A405">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B405">
-        <v>0.276003071</v>
+        <v>0.106356459</v>
       </c>
     </row>
     <row r="406">
       <c r="A406">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B406">
-        <v>0.29239983</v>
+        <v>0.106711703</v>
       </c>
     </row>
     <row r="407">
       <c r="A407">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B407">
-        <v>0.287936019</v>
+        <v>0.106042894</v>
       </c>
     </row>
     <row r="408">
       <c r="A408">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B408">
-        <v>0.304314514</v>
+        <v>0.104383383</v>
       </c>
     </row>
     <row r="409">
       <c r="A409">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B409">
-        <v>0.304748205</v>
+        <v>0.106687346</v>
       </c>
     </row>
     <row r="410">
       <c r="A410">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B410">
-        <v>0.305442274</v>
+        <v>0.104202549</v>
       </c>
     </row>
     <row r="411">
       <c r="A411">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B411">
-        <v>0.303291839</v>
+        <v>0.105969679</v>
       </c>
     </row>
     <row r="412">
       <c r="A412">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B412">
-        <v>0.312835302</v>
+        <v>0.104123319</v>
       </c>
     </row>
     <row r="413">
       <c r="A413">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="B413">
-        <v>0.314759451</v>
+        <v>0.105084417</v>
       </c>
     </row>
     <row r="414">
       <c r="A414">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B414">
-        <v>0.315194932</v>
+        <v>0.104991849</v>
       </c>
     </row>
     <row r="415">
       <c r="A415">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B415">
-        <v>0.317124592</v>
+        <v>0.110908779</v>
       </c>
     </row>
     <row r="416">
       <c r="A416">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B416">
-        <v>0.31397442</v>
+        <v>0.110923994</v>
       </c>
     </row>
     <row r="417">
       <c r="A417">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B417">
-        <v>0.315176532</v>
+        <v>0.11133904</v>
       </c>
     </row>
     <row r="418">
       <c r="A418">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="B418">
-        <v>0.318752508</v>
+        <v>0.11221669</v>
       </c>
     </row>
     <row r="419">
       <c r="A419">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="B419">
-        <v>0.321691618</v>
+        <v>0.105975999</v>
       </c>
     </row>
     <row r="420">
       <c r="A420">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B420">
-        <v>0.318373139</v>
+        <v>0.109974964</v>
       </c>
     </row>
     <row r="421">
       <c r="A421">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B421">
-        <v>0.320279367</v>
+        <v>0.112911176</v>
       </c>
     </row>
     <row r="422">
       <c r="A422">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B422">
-        <v>0.321470961</v>
+        <v>0.113640904</v>
       </c>
     </row>
     <row r="423">
       <c r="A423">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B423">
-        <v>0.323265667</v>
+        <v>0.1133071</v>
       </c>
     </row>
     <row r="424">
       <c r="A424">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B424">
-        <v>0.311891531</v>
+        <v>0.113582344</v>
       </c>
     </row>
     <row r="425">
       <c r="A425">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="B425">
-        <v>0.314682049</v>
+        <v>0.11006234</v>
       </c>
     </row>
     <row r="426">
       <c r="A426">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="B426">
-        <v>0.328795657</v>
+        <v>0.113775263</v>
       </c>
     </row>
     <row r="427">
       <c r="A427">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B427">
-        <v>0.331805141</v>
+        <v>0.114944663</v>
       </c>
     </row>
     <row r="428">
       <c r="A428">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B428">
-        <v>0.331935314</v>
+        <v>0.112987225</v>
       </c>
     </row>
     <row r="429">
       <c r="A429">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B429">
-        <v>0.317536457</v>
+        <v>0.114645521</v>
       </c>
     </row>
     <row r="430">
       <c r="A430">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B430">
-        <v>0.33501113</v>
+        <v>0.112027361</v>
       </c>
     </row>
     <row r="431">
       <c r="A431">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="B431">
-        <v>0.33469336</v>
+        <v>0.111492384</v>
       </c>
     </row>
     <row r="432">
       <c r="A432">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B432">
-        <v>0.34360363</v>
+        <v>0.112784245</v>
       </c>
     </row>
     <row r="433">
       <c r="A433">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B433">
-        <v>0.403213998</v>
+        <v>0.111909795</v>
       </c>
     </row>
     <row r="434">
       <c r="A434">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B434">
-        <v>0.41370225</v>
+        <v>0.112243933</v>
       </c>
     </row>
     <row r="435">
       <c r="A435">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B435">
-        <v>0.416450218</v>
+        <v>0.11439688</v>
       </c>
     </row>
     <row r="436">
       <c r="A436">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B436">
-        <v>0.417019832</v>
+        <v>0.114992531</v>
       </c>
     </row>
     <row r="437">
       <c r="A437">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B437">
-        <v>0.41913981</v>
+        <v>0.114541903</v>
       </c>
     </row>
     <row r="438">
       <c r="A438">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B438">
-        <v>0.408621979</v>
+        <v>0.115252126</v>
       </c>
     </row>
     <row r="439">
       <c r="A439">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B439">
-        <v>0.423646099</v>
+        <v>0.113343554</v>
       </c>
     </row>
     <row r="440">
       <c r="A440">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B440">
-        <v>0.408659071</v>
+        <v>0.101516427</v>
       </c>
     </row>
     <row r="441">
       <c r="A441">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B441">
-        <v>0.408538561</v>
+        <v>0.113769446</v>
       </c>
     </row>
     <row r="442">
       <c r="A442">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B442">
-        <v>0.422526268</v>
+        <v>0.11397645</v>
       </c>
     </row>
     <row r="443">
       <c r="A443">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B443">
-        <v>0.424774074</v>
+        <v>0.114632848</v>
       </c>
     </row>
     <row r="444">
       <c r="A444">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B444">
-        <v>0.424643317</v>
+        <v>0.113162114</v>
       </c>
     </row>
     <row r="445">
       <c r="A445">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B445">
-        <v>0.425173622</v>
+        <v>0.114502517</v>
       </c>
     </row>
     <row r="446">
       <c r="A446">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="B446">
-        <v>0.418668648</v>
+        <v>0.112501143</v>
       </c>
     </row>
     <row r="447">
       <c r="A447">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B447">
-        <v>0.422781762</v>
+        <v>0.114273559</v>
       </c>
     </row>
     <row r="448">
       <c r="A448">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B448">
-        <v>0.420565764</v>
+        <v>0.113994088</v>
       </c>
     </row>
     <row r="449">
       <c r="A449">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B449">
-        <v>0.420593599</v>
+        <v>0.11659133</v>
       </c>
     </row>
     <row r="450">
       <c r="A450">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B450">
-        <v>0.41993587</v>
+        <v>0.117203923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>